<commit_message>
Added a README file, which lists needed dependencies
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="18660" yWindow="8000" windowWidth="25360" windowHeight="18140" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="test.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140000" iterate="1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>SM</t>
   </si>
@@ -85,18 +85,33 @@
   </si>
   <si>
     <t xml:space="preserve"> K2O   </t>
+  </si>
+  <si>
+    <t>Kphase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -120,8 +135,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,15 +473,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E10"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -501,347 +521,305 @@
       <c r="N1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2">
-        <v>73.5</v>
-      </c>
-      <c r="C2">
-        <v>77.27</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="B2" s="1">
+        <v>73.495078687287759</v>
+      </c>
+      <c r="C2" s="2">
+        <v>76.248353687193699</v>
+      </c>
+      <c r="D2" s="2">
+        <v>50.503126439824584</v>
+      </c>
+      <c r="E2" s="2">
+        <v>69.767388548106794</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2">
+        <v>20.94</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B3">
-        <v>0.23300000000000001</v>
-      </c>
-      <c r="C3">
-        <v>0.15</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>7.37</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="B3" s="5">
+        <v>0.23324434510114367</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.22937065375116267</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.59771729659012562</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3.0947824000662715E-2</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="2">
+        <v>3.5344106059479166</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2">
+        <v>18.260000000000002</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4">
-        <v>11.23</v>
-      </c>
-      <c r="C4">
-        <v>11.49</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="B4" s="5">
+        <v>11.227120557711329</v>
+      </c>
+      <c r="C4" s="2">
+        <v>10.827285384443631</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.50060784269467207</v>
+      </c>
+      <c r="E4" s="2">
+        <v>18.174396198315112</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="2">
+        <v>8.0109008277105837E-3</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5">
-        <v>4.24</v>
-      </c>
-      <c r="C5">
-        <v>2.85</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>92.46</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="B5" s="5">
+        <v>4.2417996333039421</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3.5572381060308196</v>
+      </c>
+      <c r="D5" s="2">
+        <v>25.649112618528697</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="2">
+        <v>88.013333323627037</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2">
+        <v>13.41</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="C6">
-        <v>0.06</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="B6" s="5">
+        <v>8.2176762041545684E-2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>9.1398663598552338E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.2302231145494955</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2.5034392983701071E-2</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="2">
+        <v>0.79360660771616454</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7">
-        <v>0.04</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="B7" s="5">
+        <v>4.4575812888200186E-2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>7.2038355545656985E-3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.8427586889369316</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.1201653468253339E-3</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="2">
+        <v>4.5723317141901761E-2</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8">
-        <v>0.41</v>
-      </c>
-      <c r="C8">
-        <v>0.22</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="B8" s="5">
+        <v>0.41184374752994851</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.22964874299132051</v>
+      </c>
+      <c r="D8" s="2">
+        <v>15.882758092125059</v>
+      </c>
+      <c r="E8" s="2">
+        <v>8.6461134560774047E-2</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="2">
+        <v>7.1935409783864354E-2</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2">
+        <v>2.75</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9">
-        <v>5.63</v>
-      </c>
-      <c r="C9">
-        <v>4.58</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="B9" s="5">
+        <v>5.6271730070526793</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4.9003296819247018</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3.6659297060178666</v>
+      </c>
+      <c r="E9" s="2">
+        <v>8.982918520475188</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B10">
-        <v>4.62</v>
-      </c>
-      <c r="C10">
-        <v>3.38</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
+      <c r="B10" s="5">
+        <v>4.6244265651012126</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3.9091712445115583</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.11274388468676368</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2.9317332162109282</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>